<commit_message>
new figures for thesis!
</commit_message>
<xml_diff>
--- a/Data/Historical_External/DOT_Statewide.xlsx
+++ b/Data/Historical_External/DOT_Statewide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\WQ_Portal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\CL_BUD\Data\Historical_External\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487A6EDF-3639-4A02-A46B-24229981ADA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F57143-9BFC-4378-839B-0FDC71CF1B4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{86B641F3-A9FA-418A-B249-C41FC6A856B4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{86B641F3-A9FA-418A-B249-C41FC6A856B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t>Winter</t>
   </si>
   <si>
     <t>Tons</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>tons_per_lanemi</t>
   </si>
 </sst>
 </file>
@@ -402,504 +408,698 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D984577-BFD9-4E72-96CE-5EBD93FFD3C5}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1959</v>
       </c>
       <c r="B2" s="2">
         <v>93673</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="2">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1960</v>
       </c>
       <c r="B3" s="2">
         <v>54805</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="2">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1961</v>
       </c>
       <c r="B4" s="2">
         <v>109412</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="2">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1962</v>
       </c>
       <c r="B5" s="2">
         <v>77719</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="2">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>1963</v>
       </c>
       <c r="B6" s="2">
         <v>82033</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="2">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1964</v>
       </c>
       <c r="B7" s="2">
         <v>149329</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" s="2">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>1965</v>
       </c>
       <c r="B8" s="2">
         <v>111634</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="2">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>1966</v>
       </c>
       <c r="B9" s="2">
         <v>181230</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1967</v>
       </c>
       <c r="B10" s="2">
         <v>137729</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" s="2">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>1968</v>
       </c>
       <c r="B11" s="2">
         <v>193004</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" s="2">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>1969</v>
       </c>
       <c r="B12" s="2">
         <v>199353</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" s="2">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>1970</v>
       </c>
       <c r="B13" s="2">
         <v>273010</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" s="2">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>1971</v>
       </c>
       <c r="B14" s="2">
         <v>223249</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" s="2">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>1972</v>
       </c>
       <c r="B15" s="2">
         <v>256571</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>1973</v>
       </c>
       <c r="B16" s="2">
         <v>218189</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>1974</v>
       </c>
       <c r="B17" s="2">
         <v>237916</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>1975</v>
       </c>
       <c r="B18" s="2">
         <v>257154</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>1976</v>
       </c>
       <c r="B19" s="2">
         <v>188011</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>1977</v>
       </c>
       <c r="B20" s="2">
         <v>210054</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>1978</v>
       </c>
       <c r="B21" s="2">
         <v>235193</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>1979</v>
       </c>
       <c r="B22" s="2">
         <v>220180</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>1980</v>
       </c>
       <c r="B23" s="2">
         <v>151021</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>1981</v>
       </c>
       <c r="B24" s="2">
         <v>192740</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>1982</v>
       </c>
       <c r="B25" s="2">
         <v>234529</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" s="2">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>1983</v>
       </c>
       <c r="B26" s="2">
         <v>224368</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>1984</v>
       </c>
       <c r="B27" s="2">
         <v>217136</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" s="2">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>1985</v>
       </c>
       <c r="B28" s="2">
         <v>304296</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>1986</v>
       </c>
       <c r="B29" s="2">
         <v>196035</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" s="2">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>1987</v>
       </c>
       <c r="B30" s="2">
         <v>224573</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" s="2">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>1988</v>
       </c>
       <c r="B31" s="2">
         <v>230403</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" s="2">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>1989</v>
       </c>
       <c r="B32" s="2">
         <v>297004</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" s="2">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>1990</v>
       </c>
       <c r="B33" s="2">
         <v>364174</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>1991</v>
       </c>
       <c r="B34" s="2">
         <v>337079</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>1992</v>
       </c>
       <c r="B35" s="2">
         <v>416594</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" s="2">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>1993</v>
       </c>
       <c r="B36" s="2">
         <v>314489</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" s="2">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>1994</v>
       </c>
       <c r="B37" s="2">
         <v>295479</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" s="2">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>1995</v>
       </c>
       <c r="B38" s="2">
         <v>440488</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38" s="2">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>1996</v>
       </c>
       <c r="B39" s="2">
         <v>509147</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39" s="2">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>1997</v>
       </c>
       <c r="B40" s="2">
         <v>413824</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>1998</v>
       </c>
       <c r="B41" s="2">
         <v>371602</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41" s="2">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>1999</v>
       </c>
       <c r="B42" s="2">
         <v>346963</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42" s="2">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>2000</v>
       </c>
       <c r="B43" s="2">
         <v>521056</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43" s="2">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>2001</v>
       </c>
       <c r="B44" s="2">
         <v>308954</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>2002</v>
       </c>
       <c r="B45" s="2">
         <v>328922</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45" s="2">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>2003</v>
       </c>
       <c r="B46" s="2">
         <v>390664</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46" s="2">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>2004</v>
       </c>
       <c r="B47" s="2">
         <v>407924</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47" s="2">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>2005</v>
       </c>
       <c r="B48" s="2">
         <v>410570</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48" s="2">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>2006</v>
       </c>
       <c r="B49" s="2">
         <v>405793</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49" s="2">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>2007</v>
       </c>
       <c r="B50" s="2">
         <v>644484</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50" s="2">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>2008</v>
       </c>
       <c r="B51" s="2">
         <v>569985</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>2009</v>
       </c>
       <c r="B52" s="2">
         <v>408523</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52" s="2">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>2010</v>
       </c>
       <c r="B53" s="2">
         <v>573253</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>2011</v>
       </c>
       <c r="B54" s="2">
         <v>355519</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54" s="2">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>2012</v>
       </c>
       <c r="B55" s="2">
         <v>621207</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55" s="2">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>2013</v>
       </c>
       <c r="B56" s="2">
         <v>669807</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56" s="2">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>2014</v>
       </c>
       <c r="B57" s="2">
         <v>388797</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57" s="2">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>2015</v>
       </c>
       <c r="B58" s="2">
         <v>399045.87999999989</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58" s="2">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>2016</v>
       </c>
       <c r="B59" s="2">
         <v>526198</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59" s="2">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>2017</v>
       </c>
       <c r="B60" s="2">
         <v>567599.61327056005</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C60" s="2">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>2018</v>
       </c>
       <c r="B61" s="2">
         <v>553442.71192035056</v>
+      </c>
+      <c r="C61" s="2">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B62" s="2">
+        <v>425558</v>
+      </c>
+      <c r="C62" s="2">
+        <v>12.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>